<commit_message>
Completed Deck for 2019 US Symposium
</commit_message>
<xml_diff>
--- a/materials/Usagi/DUTCH_ICPC_CONDITION_CODES_TO_MAP.xlsx
+++ b/materials/Usagi/DUTCH_ICPC_CONDITION_CODES_TO_MAP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\GitHub\Tutorial-ETL\materials\Usagi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B00783-3D60-410C-B5DA-4AE3326F8497}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDEA46B-239B-4766-9710-DBBC2A81DA12}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="8085" xr2:uid="{F391782D-0378-417B-8857-433FF883579C}"/>
+    <workbookView xWindow="-26460" yWindow="2340" windowWidth="21600" windowHeight="11505" xr2:uid="{F391782D-0378-417B-8857-433FF883579C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>ICPC_CODE</t>
   </si>
@@ -110,10 +110,10 @@
     <t>Acute pharyngitis</t>
   </si>
   <si>
-    <t>ICPC_DESCRIPTION_ENGLIGH</t>
-  </si>
-  <si>
     <t>ICPC_DESCRIPTION_DUTCH</t>
+  </si>
+  <si>
+    <t>ICPC_DESCRIPTION_ENGLISH</t>
   </si>
 </sst>
 </file>
@@ -469,7 +469,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,10 +485,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
         <v>27</v>
-      </c>
-      <c r="C1" t="s">
-        <v>26</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>

</xml_diff>